<commit_message>
labs tweak, benchmark spreadsheet tweak [1:00]
</commit_message>
<xml_diff>
--- a/04-dataframe/Benchmarking_Dataformats.xlsx
+++ b/04-dataframe/Benchmarking_Dataformats.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27907"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28702"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sujee/ElephantScale/spark-labs/05-sql/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sujee/ElephantScale/spark-labs/04-dataframe/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="560" yWindow="560" windowWidth="27900" windowHeight="18500" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="560" yWindow="460" windowWidth="27900" windowHeight="16440" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
-    <sheet name="sample results" sheetId="4" r:id="rId2"/>
+    <sheet name="sample results (read only)" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -90,6 +90,7 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -122,6 +123,7 @@
       <sz val="18"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -130,6 +132,7 @@
       <sz val="20"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -402,11 +405,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-65164912"/>
-        <c:axId val="-65162592"/>
+        <c:axId val="1956315712"/>
+        <c:axId val="1946258864"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-65164912"/>
+        <c:axId val="1956315712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -416,7 +419,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-65162592"/>
+        <c:crossAx val="1946258864"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -424,7 +427,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-65162592"/>
+        <c:axId val="1946258864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -435,7 +438,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-65164912"/>
+        <c:crossAx val="1956315712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -528,11 +531,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-195417952"/>
-        <c:axId val="-195408256"/>
+        <c:axId val="1956334992"/>
+        <c:axId val="1956207552"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-195417952"/>
+        <c:axId val="1956334992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -542,7 +545,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-195408256"/>
+        <c:crossAx val="1956207552"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -550,7 +553,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-195408256"/>
+        <c:axId val="1956207552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -561,7 +564,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-195417952"/>
+        <c:crossAx val="1956334992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -665,11 +668,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-195379696"/>
-        <c:axId val="-195370720"/>
+        <c:axId val="1942427952"/>
+        <c:axId val="1891585808"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-195379696"/>
+        <c:axId val="1942427952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -679,7 +682,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-195370720"/>
+        <c:crossAx val="1891585808"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -687,7 +690,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-195370720"/>
+        <c:axId val="1891585808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -698,7 +701,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-195379696"/>
+        <c:crossAx val="1942427952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -812,11 +815,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-195337696"/>
-        <c:axId val="-195335376"/>
+        <c:axId val="1956730512"/>
+        <c:axId val="1945297072"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-195337696"/>
+        <c:axId val="1956730512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -859,7 +862,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-195335376"/>
+        <c:crossAx val="1945297072"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -867,7 +870,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-195335376"/>
+        <c:axId val="1945297072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -917,7 +920,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-195337696"/>
+        <c:crossAx val="1956730512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1002,7 +1005,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'sample results'!$B$4</c:f>
+              <c:f>'sample results (read only)'!$B$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1014,7 +1017,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'sample results'!$A$5:$A$8</c:f>
+              <c:f>'sample results (read only)'!$A$5:$A$8</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -1034,7 +1037,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'sample results'!$B$5:$B$8</c:f>
+              <c:f>'sample results (read only)'!$B$5:$B$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1063,11 +1066,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-67053344"/>
-        <c:axId val="-67012784"/>
+        <c:axId val="1951706944"/>
+        <c:axId val="1887356000"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-67053344"/>
+        <c:axId val="1951706944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1077,7 +1080,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-67012784"/>
+        <c:crossAx val="1887356000"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1085,7 +1088,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-67012784"/>
+        <c:axId val="1887356000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1096,7 +1099,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-67053344"/>
+        <c:crossAx val="1951706944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1140,7 +1143,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'sample results'!$A$13:$A$16</c:f>
+              <c:f>'sample results (read only)'!$A$13:$A$16</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -1160,7 +1163,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'sample results'!$B$13:$B$16</c:f>
+              <c:f>'sample results (read only)'!$B$13:$B$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1189,11 +1192,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-60554656"/>
-        <c:axId val="-60552336"/>
+        <c:axId val="1951734128"/>
+        <c:axId val="1954110752"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-60554656"/>
+        <c:axId val="1951734128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1203,7 +1206,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-60552336"/>
+        <c:crossAx val="1954110752"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1211,7 +1214,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-60552336"/>
+        <c:axId val="1954110752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1222,7 +1225,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-60554656"/>
+        <c:crossAx val="1951734128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1265,7 +1268,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'sample results'!$C$26</c:f>
+              <c:f>'sample results (read only)'!$C$26</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1277,7 +1280,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'sample results'!$A$27:$A$30</c:f>
+              <c:f>'sample results (read only)'!$A$27:$A$30</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -1297,7 +1300,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'sample results'!$C$27:$C$30</c:f>
+              <c:f>'sample results (read only)'!$C$27:$C$30</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1326,11 +1329,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-60534160"/>
-        <c:axId val="-60531840"/>
+        <c:axId val="1951099056"/>
+        <c:axId val="1958814944"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-60534160"/>
+        <c:axId val="1951099056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1340,7 +1343,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-60531840"/>
+        <c:crossAx val="1958814944"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1348,7 +1351,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-60531840"/>
+        <c:axId val="1958814944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1359,7 +1362,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-60534160"/>
+        <c:crossAx val="1951099056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1412,7 +1415,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'sample results'!$A$21:$A$22</c:f>
+              <c:f>'sample results (read only)'!$A$21:$A$22</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
@@ -1426,7 +1429,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'sample results'!$B$21:$B$22</c:f>
+              <c:f>'sample results (read only)'!$B$21:$B$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
@@ -1450,11 +1453,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-57982416"/>
-        <c:axId val="-57980640"/>
+        <c:axId val="1950999264"/>
+        <c:axId val="1950550256"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-57982416"/>
+        <c:axId val="1950999264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1497,7 +1500,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-57980640"/>
+        <c:crossAx val="1950550256"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1505,7 +1508,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-57980640"/>
+        <c:axId val="1950550256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1556,7 +1559,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-57982416"/>
+        <c:crossAx val="1950999264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3268,7 +3271,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:D30"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
@@ -3516,8 +3519,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+    <sheetView topLeftCell="A2" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3737,6 +3740,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>

</xml_diff>